<commit_message>
Atualizaçao Sprint Backlog e Documento Final V2
</commit_message>
<xml_diff>
--- a/Docs/Sprint Backlog com Casos de Uso.xlsx
+++ b/Docs/Sprint Backlog com Casos de Uso.xlsx
@@ -525,7 +525,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,6 +561,15 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -570,7 +579,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -614,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,12 +633,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -657,9 +660,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,12 +1017,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1029,66 +1039,66 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1"/>
@@ -1097,10 +1107,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="1"/>
@@ -1109,7 +1119,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1121,21 +1131,21 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1147,10 +1157,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="3">
@@ -1161,7 +1171,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1173,10 +1183,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="1"/>
@@ -1185,7 +1195,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1197,10 +1207,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3">
@@ -1210,8 +1220,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1222,11 +1232,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3">
@@ -1236,8 +1246,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="5"/>
@@ -1246,8 +1256,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="5"/>
@@ -1256,8 +1266,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1268,22 +1278,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+    <row r="22" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1294,8 +1304,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1305,35 +1315,36 @@
       <c r="D24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="16"/>
+      <c r="C25" s="14"/>
       <c r="D25" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1344,22 +1355,22 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="3">
         <v>4</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1368,8 +1379,8 @@
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1378,8 +1389,8 @@
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1388,8 +1399,8 @@
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1397,13 +1408,13 @@
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>